<commit_message>
Added BLEU metric (WIP)
</commit_message>
<xml_diff>
--- a/Translations/Translations_Julie.xlsx
+++ b/Translations/Translations_Julie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konst/Documents/GitHub/data-wild-west/Translations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/gifa_itu_dk/Documents/Documents/GitHub/data-wild-west/Translations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3355E6DD-D772-9B43-9BD1-C33D609AC2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{3355E6DD-D772-9B43-9BD1-C33D609AC2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{239A7757-2771-4CEC-8E42-53570CA79938}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{FB25DA82-F7CF-441D-B825-4E339B81093A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FB25DA82-F7CF-441D-B825-4E339B81093A}"/>
   </bookViews>
   <sheets>
     <sheet name="Trans.3" sheetId="1" r:id="rId1"/>
@@ -200,13 +200,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,48 +524,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9BAF3A-7C9C-4AFB-9C58-5D1A7633A20A}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="129.6640625" customWidth="1"/>
-    <col min="2" max="2" width="74.33203125" style="5" customWidth="1"/>
-    <col min="3" max="12" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="129.7109375" customWidth="1"/>
+    <col min="2" max="2" width="74.28515625" style="3" customWidth="1"/>
+    <col min="3" max="12" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="3" t="s">
+      <c r="L1" s="4"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -599,11 +599,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C3" t="s">
@@ -616,33 +616,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
@@ -655,11 +655,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
@@ -672,11 +672,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C8" t="s">
@@ -689,11 +689,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F9" t="s">
@@ -703,11 +703,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
@@ -720,11 +720,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D11" t="s">
@@ -737,11 +737,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
       <c r="E12" t="s">
@@ -757,11 +757,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F13" t="s">
@@ -771,33 +771,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D16" t="s">
@@ -810,11 +810,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
@@ -824,49 +824,49 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
     </row>
   </sheetData>

</xml_diff>